<commit_message>
calcul pire temps pire backlog
</commit_message>
<xml_diff>
--- a/calculsNetworkCalculus.xlsx
+++ b/calculsNetworkCalculus.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>a</t>
   </si>
@@ -69,6 +69,66 @@
   </si>
   <si>
     <t>Coef Courbes d'arrivée :</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>B31</t>
+  </si>
+  <si>
+    <t>B41</t>
+  </si>
+  <si>
+    <t>B51</t>
+  </si>
+  <si>
+    <t>B22</t>
+  </si>
+  <si>
+    <t>Flux</t>
+  </si>
+  <si>
+    <t>tau (ms)</t>
+  </si>
+  <si>
+    <t>tau (us)</t>
+  </si>
+  <si>
+    <t>mu (octet)</t>
+  </si>
+  <si>
+    <t>WCTT</t>
+  </si>
+  <si>
+    <t>vl</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>v3</t>
+  </si>
+  <si>
+    <t>v4</t>
+  </si>
+  <si>
+    <t>v5</t>
   </si>
 </sst>
 </file>
@@ -114,7 +174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -190,11 +250,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -204,6 +310,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,14 +630,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
@@ -690,6 +803,216 @@
         <v>1547</v>
       </c>
     </row>
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="10">
+        <f>367/12500</f>
+        <v>2.9360000000000001E-2</v>
+      </c>
+      <c r="C11" s="5">
+        <f>B11*1000</f>
+        <v>29.36</v>
+      </c>
+      <c r="D11" s="3">
+        <f>21042/125</f>
+        <v>168.33600000000001</v>
+      </c>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="9">
+        <f>1047/12500</f>
+        <v>8.3760000000000001E-2</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" ref="C12:C19" si="3">B12*1000</f>
+        <v>83.76</v>
+      </c>
+      <c r="D12" s="4">
+        <f>2648198/3125</f>
+        <v>847.42336</v>
+      </c>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="9">
+        <f>367/12500</f>
+        <v>2.9360000000000001E-2</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" si="3"/>
+        <v>29.36</v>
+      </c>
+      <c r="D13" s="4">
+        <f>21042/125</f>
+        <v>168.33600000000001</v>
+      </c>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="9">
+        <f>1047/12500</f>
+        <v>8.3760000000000001E-2</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" si="3"/>
+        <v>83.76</v>
+      </c>
+      <c r="D14" s="4">
+        <f>105928/125</f>
+        <v>847.42399999999998</v>
+      </c>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="9">
+        <f>23021/781250</f>
+        <v>2.9466880000000001E-2</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" si="3"/>
+        <v>29.46688</v>
+      </c>
+      <c r="D15" s="4">
+        <f>21209/125</f>
+        <v>169.672</v>
+      </c>
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="9">
+        <f>23021/781250</f>
+        <v>2.9466880000000001E-2</v>
+      </c>
+      <c r="C16" s="6">
+        <f t="shared" si="3"/>
+        <v>29.46688</v>
+      </c>
+      <c r="D16" s="4">
+        <f>21209/125</f>
+        <v>169.672</v>
+      </c>
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="9">
+        <f>32732/390625</f>
+        <v>8.3793919999999994E-2</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="3"/>
+        <v>83.79392</v>
+      </c>
+      <c r="D17" s="4">
+        <f>105981/125</f>
+        <v>847.84799999999996</v>
+      </c>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="9">
+        <f>1747/12500</f>
+        <v>0.13976</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" si="3"/>
+        <v>139.76</v>
+      </c>
+      <c r="D18" s="4">
+        <f>966996/625</f>
+        <v>1547.1936000000001</v>
+      </c>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="11">
+        <f>1636599/19531250</f>
+        <v>8.3793868800000004E-2</v>
+      </c>
+      <c r="C19" s="7">
+        <f t="shared" si="3"/>
+        <v>83.793868799999998</v>
+      </c>
+      <c r="D19" s="8">
+        <f>2649521/3125</f>
+        <v>847.84672</v>
+      </c>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Il reste a faire :
* Relecture générale faute de frappe gnagnagna 
* Conclusion fin du chap 2 : générale + amélioration de la sérialisation 
* CHAPITRE 3 : la question 1 à l'air easy, jette un oeil si t'as le temps
* L'intro 
* Annexe Le script network calc + l'excel
* Dormir !!!!
</commit_message>
<xml_diff>
--- a/calculsNetworkCalculus.xlsx
+++ b/calculsNetworkCalculus.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
   <si>
     <t>a</t>
   </si>
@@ -153,6 +153,27 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>mu (octets)</t>
+  </si>
+  <si>
+    <t>nœuds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comparaison mu </t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -237,7 +258,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -418,6 +439,34 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -443,8 +492,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -457,6 +504,8 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -772,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" zoomScale="70" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="70" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +833,7 @@
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="28.44140625" customWidth="1"/>
     <col min="5" max="5" width="30.77734375" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -946,16 +995,16 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
     </row>
     <row r="10" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -967,7 +1016,12 @@
       <c r="D10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="12"/>
+      <c r="E10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
@@ -985,7 +1039,13 @@
         <f>21042/125</f>
         <v>168.33600000000001</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="5">
+        <f>D11+D12</f>
+        <v>1015.75936</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
@@ -1003,7 +1063,8 @@
         <f>2648198/3125</f>
         <v>847.42336</v>
       </c>
-      <c r="E12" s="11"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
@@ -1021,7 +1082,13 @@
         <f>21042/125</f>
         <v>168.33600000000001</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="6">
+        <f>D13+D14</f>
+        <v>1015.76</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
@@ -1039,7 +1106,8 @@
         <f>105928/125</f>
         <v>847.42399999999998</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
@@ -1057,7 +1125,13 @@
         <f>21209/125</f>
         <v>169.672</v>
       </c>
-      <c r="E15" s="11"/>
+      <c r="E15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="6">
+        <f>SUM(D15:D19)</f>
+        <v>3582.2323200000001</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
@@ -1075,9 +1149,10 @@
         <f>21209/125</f>
         <v>169.672</v>
       </c>
-      <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
@@ -1093,9 +1168,10 @@
         <f>105981/125</f>
         <v>847.84799999999996</v>
       </c>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>22</v>
       </c>
@@ -1111,9 +1187,10 @@
         <f>966996/625</f>
         <v>1547.1936000000001</v>
       </c>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>23</v>
       </c>
@@ -1129,27 +1206,35 @@
         <f>2649521/3125</f>
         <v>847.84672</v>
       </c>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="18" t="s">
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="19">
+      <c r="B20" s="17">
         <f>MAX(B11:B19)</f>
         <v>0.13976</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="18">
         <f t="shared" ref="C20:D20" si="4">MAX(C11:C19)</f>
         <v>139.76</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="19">
         <f t="shared" si="4"/>
         <v>1547.1936000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
+      <c r="E20" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="24">
+        <f>MAX(F11:F15)</f>
+        <v>3582.2323200000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1159,7 +1244,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>29</v>
       </c>
@@ -1172,7 +1257,7 @@
         <v>58.826880000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>30</v>
       </c>
@@ -1185,7 +1270,7 @@
         <v>167.5538688</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>31</v>
       </c>
@@ -1198,7 +1283,7 @@
         <v>58.826880000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>32</v>
       </c>
@@ -1211,7 +1296,7 @@
         <v>167.55392000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>33</v>
       </c>
@@ -1224,33 +1309,33 @@
         <v>139.76</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="22" t="s">
+    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="23">
+      <c r="B29" s="21">
         <f>MAX(B24:B28)</f>
         <v>0.16755392</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="22">
         <f>MAX(C24:C28)</f>
         <v>167.55392000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C30" s="16"/>
-    </row>
-    <row r="31" spans="1:5" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="14" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-    </row>
-    <row r="32" spans="1:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13" t="s">
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+    </row>
+    <row r="32" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1262,8 +1347,14 @@
       <c r="D32" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>15</v>
       </c>
@@ -1279,11 +1370,18 @@
         <f>21042/125</f>
         <v>168.33600000000001</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="5">
+        <f>D33+D34</f>
+        <v>1015.75936</v>
+      </c>
+      <c r="G33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>16</v>
       </c>
@@ -1299,11 +1397,13 @@
         <f>2648198/3125</f>
         <v>847.42336</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>38</v>
       </c>
@@ -1319,8 +1419,15 @@
         <f>25394/25</f>
         <v>1015.76</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="6">
+        <f>D35</f>
+        <v>1015.76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>19</v>
       </c>
@@ -1336,11 +1443,18 @@
         <f>21209/125</f>
         <v>169.672</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" s="6">
+        <f>SUM(D37:D39)</f>
+        <v>2595.0403200000001</v>
+      </c>
+      <c r="G36" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>39</v>
       </c>
@@ -1356,8 +1470,10 @@
         <f>200</f>
         <v>200</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>22</v>
       </c>
@@ -1373,11 +1489,13 @@
         <f>966996/625</f>
         <v>1547.1936000000001</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>23</v>
       </c>
@@ -1393,32 +1511,41 @@
         <f>2649521/3125</f>
         <v>847.84672</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="18" t="s">
+    <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="19">
+      <c r="B40" s="17">
         <f>MAX(B33:B39)</f>
         <v>0.13976</v>
       </c>
-      <c r="C40" s="20">
+      <c r="C40" s="18">
         <f t="shared" ref="C40:D40" si="6">MAX(C33:C39)</f>
         <v>139.76</v>
       </c>
-      <c r="D40" s="21">
+      <c r="D40" s="19">
         <f t="shared" si="6"/>
         <v>1547.1936000000001</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E40" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" s="24">
+        <f>MAX(F33:F36)</f>
+        <v>2595.0403200000001</v>
+      </c>
+      <c r="G40" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="13" t="s">
+    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1428,7 +1555,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>29</v>
       </c>
@@ -1444,7 +1571,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>30</v>
       </c>
@@ -1460,7 +1587,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>31</v>
       </c>
@@ -1473,7 +1600,7 @@
         <v>113.12</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>32</v>
       </c>
@@ -1486,7 +1613,7 @@
         <v>113.12</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
         <v>33</v>
       </c>
@@ -1502,20 +1629,34 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="18" t="s">
+    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B48" s="20">
+      <c r="B48" s="18">
         <f>MAX(B43:B47)</f>
         <v>0.16755386880000001</v>
       </c>
-      <c r="C48" s="21">
+      <c r="C48" s="19">
         <f>MAX(C43:C47)</f>
         <v>167.5538688</v>
       </c>
-      <c r="D48" s="17" t="s">
+      <c r="D48" s="15" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <f>(F40-F20)/F40*100</f>
+        <v>-38.041489852458241</v>
+      </c>
+      <c r="B52" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>